<commit_message>
Update System, removed inverter
</commit_message>
<xml_diff>
--- a/SA_Capacity_Costs/SA_Capacity_Costs_HPHB.xlsx
+++ b/SA_Capacity_Costs/SA_Capacity_Costs_HPHB.xlsx
@@ -521,22 +521,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6.8285</v>
+        <v>6.87565</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9774</v>
+        <v>1.2232</v>
       </c>
       <c r="D2" t="n">
-        <v>35.58035</v>
+        <v>35.04514999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.0359</v>
       </c>
       <c r="F2" t="n">
-        <v>28.18565000000001</v>
+        <v>26.92725</v>
       </c>
       <c r="G2" t="n">
-        <v>28.18565000000001</v>
+        <v>26.92725</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -548,19 +548,19 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>62.761</v>
+        <v>67.2974</v>
       </c>
       <c r="L2" t="n">
-        <v>28.186</v>
+        <v>26.927</v>
       </c>
       <c r="M2" t="n">
-        <v>34.575</v>
+        <v>40.3704</v>
       </c>
       <c r="N2" t="n">
-        <v>7.780199999999999</v>
+        <v>7.785999999999999</v>
       </c>
       <c r="O2" t="n">
-        <v>26.7948</v>
+        <v>32.5844</v>
       </c>
     </row>
     <row r="3">
@@ -570,43 +570,43 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12.011</v>
+        <v>12.049</v>
       </c>
       <c r="C3" t="n">
-        <v>3.524</v>
+        <v>3.54</v>
       </c>
       <c r="D3" t="n">
-        <v>53.563</v>
+        <v>53.524</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>32.2</v>
+        <v>30.926</v>
       </c>
       <c r="G3" t="n">
-        <v>30.469</v>
+        <v>29.193</v>
       </c>
       <c r="H3" t="n">
-        <v>1.73</v>
+        <v>1.733</v>
       </c>
       <c r="I3" t="n">
-        <v>1.73</v>
+        <v>1.733</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>33.7062</v>
+        <v>32.437</v>
       </c>
       <c r="L3" t="n">
-        <v>30.469</v>
+        <v>29.193</v>
       </c>
       <c r="M3" t="n">
-        <v>3.2372</v>
+        <v>3.244</v>
       </c>
       <c r="N3" t="n">
-        <v>3.2372</v>
+        <v>3.244</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
@@ -619,22 +619,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>33.227</v>
+        <v>33.529</v>
       </c>
       <c r="C4" t="n">
-        <v>1.978</v>
+        <v>2.449</v>
       </c>
       <c r="D4" t="n">
-        <v>54.428</v>
+        <v>53.46</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>37.056</v>
+        <v>35.893</v>
       </c>
       <c r="G4" t="n">
-        <v>37.05590136986302</v>
+        <v>35.8925808219178</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -646,10 +646,10 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>37.056</v>
+        <v>35.893</v>
       </c>
       <c r="L4" t="n">
-        <v>37.056</v>
+        <v>35.893</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -764,22 +764,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6.15235</v>
+        <v>6.19875</v>
       </c>
       <c r="C2" t="n">
-        <v>0.93665</v>
+        <v>1.20455</v>
       </c>
       <c r="D2" t="n">
-        <v>35.22055</v>
+        <v>34.63824999999999</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.0359</v>
       </c>
       <c r="F2" t="n">
-        <v>27.95940000000001</v>
+        <v>26.70205</v>
       </c>
       <c r="G2" t="n">
-        <v>27.95940000000001</v>
+        <v>26.70205</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -791,19 +791,19 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>243.0678</v>
+        <v>229.8882</v>
       </c>
       <c r="L2" t="n">
-        <v>27.959</v>
+        <v>26.70200000000001</v>
       </c>
       <c r="M2" t="n">
-        <v>215.1088</v>
+        <v>203.1862</v>
       </c>
       <c r="N2" t="n">
-        <v>8.942</v>
+        <v>8.9472</v>
       </c>
       <c r="O2" t="n">
-        <v>206.1668</v>
+        <v>194.2392</v>
       </c>
     </row>
     <row r="3">
@@ -813,46 +813,46 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9.052</v>
+        <v>9.163</v>
       </c>
       <c r="C3" t="n">
-        <v>3.811</v>
+        <v>3.818</v>
       </c>
       <c r="D3" t="n">
-        <v>53.424</v>
+        <v>53.394</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>31.066</v>
+        <v>29.79</v>
       </c>
       <c r="G3" t="n">
-        <v>29.558</v>
+        <v>28.304</v>
       </c>
       <c r="H3" t="n">
-        <v>1.509</v>
+        <v>1.486</v>
       </c>
       <c r="I3" t="n">
-        <v>1.509</v>
+        <v>1.486</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>113.992</v>
+        <v>109.947</v>
       </c>
       <c r="L3" t="n">
-        <v>29.558</v>
+        <v>28.30399999999999</v>
       </c>
       <c r="M3" t="n">
-        <v>84.434</v>
+        <v>81.643</v>
       </c>
       <c r="N3" t="n">
-        <v>7.8334</v>
+        <v>7.8102</v>
       </c>
       <c r="O3" t="n">
-        <v>76.6006</v>
+        <v>73.83279999999999</v>
       </c>
     </row>
     <row r="4">
@@ -862,22 +862,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>19.701</v>
+        <v>19.899</v>
       </c>
       <c r="C4" t="n">
-        <v>2.777</v>
+        <v>2.786</v>
       </c>
       <c r="D4" t="n">
-        <v>53.925</v>
+        <v>53.876</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>32.838</v>
+        <v>31.612</v>
       </c>
       <c r="G4" t="n">
-        <v>32.83793698630137</v>
+        <v>31.61164383561644</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -889,16 +889,16 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>36.2944</v>
+        <v>35.071</v>
       </c>
       <c r="L4" t="n">
-        <v>32.838</v>
+        <v>31.612</v>
       </c>
       <c r="M4" t="n">
-        <v>3.4564</v>
+        <v>3.459000000000001</v>
       </c>
       <c r="N4" t="n">
-        <v>3.4564</v>
+        <v>3.459000000000001</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
@@ -1007,22 +1007,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.656700000000003</v>
+        <v>7.723350000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>1.08965</v>
+        <v>1.3063</v>
       </c>
       <c r="D2" t="n">
-        <v>33.1677</v>
+        <v>32.7205</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>28.4108</v>
+        <v>27.15645</v>
       </c>
       <c r="G2" t="n">
-        <v>28.4108</v>
+        <v>27.15645</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -1034,19 +1034,19 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>84.0228</v>
+        <v>77.2728</v>
       </c>
       <c r="L2" t="n">
-        <v>28.411</v>
+        <v>27.156</v>
       </c>
       <c r="M2" t="n">
-        <v>55.6118</v>
+        <v>50.1168</v>
       </c>
       <c r="N2" t="n">
-        <v>5.8288</v>
+        <v>5.8988</v>
       </c>
       <c r="O2" t="n">
-        <v>49.7832</v>
+        <v>44.218</v>
       </c>
     </row>
     <row r="3">
@@ -1056,37 +1056,37 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12.011</v>
+        <v>12.049</v>
       </c>
       <c r="C3" t="n">
-        <v>3.524</v>
+        <v>3.54</v>
       </c>
       <c r="D3" t="n">
-        <v>53.563</v>
+        <v>53.524</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>33.009</v>
+        <v>31.738</v>
       </c>
       <c r="G3" t="n">
-        <v>30.469</v>
+        <v>29.193</v>
       </c>
       <c r="H3" t="n">
-        <v>2.54</v>
+        <v>2.544</v>
       </c>
       <c r="I3" t="n">
-        <v>2.54</v>
+        <v>2.544</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>30.469</v>
+        <v>29.193</v>
       </c>
       <c r="L3" t="n">
-        <v>30.469</v>
+        <v>29.193</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -1105,22 +1105,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>33.227</v>
+        <v>33.529</v>
       </c>
       <c r="C4" t="n">
-        <v>1.978</v>
+        <v>2.449</v>
       </c>
       <c r="D4" t="n">
-        <v>54.428</v>
+        <v>53.46</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>37.056</v>
+        <v>35.893</v>
       </c>
       <c r="G4" t="n">
-        <v>37.05590136986302</v>
+        <v>35.8925808219178</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -1132,10 +1132,10 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>37.056</v>
+        <v>35.893</v>
       </c>
       <c r="L4" t="n">
-        <v>37.056</v>
+        <v>35.893</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -1250,22 +1250,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8.227700000000002</v>
+        <v>8.298950000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>1.13765</v>
+        <v>1.2959</v>
       </c>
       <c r="D2" t="n">
-        <v>33.19575</v>
+        <v>32.83895</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.0359</v>
       </c>
       <c r="F2" t="n">
-        <v>28.59765</v>
+        <v>27.3412</v>
       </c>
       <c r="G2" t="n">
-        <v>28.59765</v>
+        <v>27.3412</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -1277,19 +1277,19 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>34.0072</v>
+        <v>47.029</v>
       </c>
       <c r="L2" t="n">
-        <v>28.598</v>
+        <v>27.341</v>
       </c>
       <c r="M2" t="n">
-        <v>5.409199999999999</v>
+        <v>19.688</v>
       </c>
       <c r="N2" t="n">
-        <v>2.7584</v>
+        <v>2.7378</v>
       </c>
       <c r="O2" t="n">
-        <v>2.6508</v>
+        <v>16.9502</v>
       </c>
     </row>
     <row r="3">
@@ -1299,37 +1299,37 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12.011</v>
+        <v>12.049</v>
       </c>
       <c r="C3" t="n">
-        <v>3.524</v>
+        <v>3.54</v>
       </c>
       <c r="D3" t="n">
-        <v>53.563</v>
+        <v>53.524</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>33.009</v>
+        <v>31.738</v>
       </c>
       <c r="G3" t="n">
-        <v>30.469</v>
+        <v>29.193</v>
       </c>
       <c r="H3" t="n">
-        <v>2.54</v>
+        <v>2.544</v>
       </c>
       <c r="I3" t="n">
-        <v>2.54</v>
+        <v>2.544</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>30.469</v>
+        <v>29.193</v>
       </c>
       <c r="L3" t="n">
-        <v>30.469</v>
+        <v>29.193</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -1348,22 +1348,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>33.227</v>
+        <v>33.529</v>
       </c>
       <c r="C4" t="n">
-        <v>1.978</v>
+        <v>2.449</v>
       </c>
       <c r="D4" t="n">
-        <v>54.428</v>
+        <v>53.46</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>37.056</v>
+        <v>35.893</v>
       </c>
       <c r="G4" t="n">
-        <v>37.05590136986302</v>
+        <v>35.8925808219178</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -1375,10 +1375,10 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>37.056</v>
+        <v>35.893</v>
       </c>
       <c r="L4" t="n">
-        <v>37.056</v>
+        <v>35.893</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -1493,22 +1493,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.97115</v>
+        <v>8.0367</v>
       </c>
       <c r="C2" t="n">
-        <v>0.89345</v>
+        <v>1.05765</v>
       </c>
       <c r="D2" t="n">
-        <v>34.04925</v>
+        <v>33.68215</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.0359</v>
       </c>
       <c r="F2" t="n">
-        <v>28.5079</v>
+        <v>27.25005000000001</v>
       </c>
       <c r="G2" t="n">
-        <v>28.5079</v>
+        <v>27.25005000000001</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -1520,19 +1520,19 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>134.3444</v>
+        <v>145.9106</v>
       </c>
       <c r="L2" t="n">
-        <v>28.508</v>
+        <v>27.25</v>
       </c>
       <c r="M2" t="n">
-        <v>105.8364</v>
+        <v>118.6606</v>
       </c>
       <c r="N2" t="n">
-        <v>3.1986</v>
+        <v>3.2118</v>
       </c>
       <c r="O2" t="n">
-        <v>102.6376</v>
+        <v>115.4488</v>
       </c>
     </row>
     <row r="3">
@@ -1542,46 +1542,46 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12.027</v>
+        <v>12.081</v>
       </c>
       <c r="C3" t="n">
-        <v>2.27</v>
+        <v>2.901</v>
       </c>
       <c r="D3" t="n">
-        <v>53.313</v>
+        <v>52.019</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>32.871</v>
+        <v>31.645</v>
       </c>
       <c r="G3" t="n">
-        <v>30.336</v>
+        <v>29.105</v>
       </c>
       <c r="H3" t="n">
-        <v>2.534</v>
+        <v>2.54</v>
       </c>
       <c r="I3" t="n">
-        <v>2.534</v>
+        <v>2.54</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>61.83459999999999</v>
+        <v>42.3792</v>
       </c>
       <c r="L3" t="n">
-        <v>30.337</v>
+        <v>29.105</v>
       </c>
       <c r="M3" t="n">
-        <v>31.4976</v>
+        <v>13.2742</v>
       </c>
       <c r="N3" t="n">
-        <v>0.2966</v>
+        <v>0.2958</v>
       </c>
       <c r="O3" t="n">
-        <v>31.2012</v>
+        <v>12.9786</v>
       </c>
     </row>
     <row r="4">
@@ -1591,22 +1591,22 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>33.278</v>
+        <v>33.529</v>
       </c>
       <c r="C4" t="n">
-        <v>1.705</v>
+        <v>2.449</v>
       </c>
       <c r="D4" t="n">
-        <v>54.473</v>
+        <v>52.947</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>37.044</v>
+        <v>35.882</v>
       </c>
       <c r="G4" t="n">
-        <v>37.04413424657535</v>
+        <v>35.88203287671233</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -1618,19 +1618,19 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>45.0732</v>
+        <v>35.926</v>
       </c>
       <c r="L4" t="n">
-        <v>37.044</v>
+        <v>35.882</v>
       </c>
       <c r="M4" t="n">
-        <v>8.029199999999999</v>
+        <v>0.044</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0442</v>
+        <v>0.044</v>
       </c>
       <c r="O4" t="n">
-        <v>7.985200000000001</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>